<commit_message>
Attention - a bit better
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="57">
   <si>
     <t>Experiment 1</t>
   </si>
@@ -171,13 +171,37 @@
   </si>
   <si>
     <t>result Dropout(0.2)</t>
+  </si>
+  <si>
+    <t>tail</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>Experiment 6</t>
+  </si>
+  <si>
+    <t>Experiment 7</t>
+  </si>
+  <si>
+    <t>categorical_accuracy</t>
+  </si>
+  <si>
+    <t>unit_num</t>
+  </si>
+  <si>
+    <t>#units</t>
+  </si>
+  <si>
+    <t>Experiment 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,13 +240,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +282,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -261,12 +297,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,25 +355,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -615,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S85"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,7 +1604,7 @@
         <v>29</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="I36" s="23"/>
       <c r="J36" s="1"/>
@@ -1966,7 +2006,7 @@
         <v>29</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2109,9 +2149,7 @@
       <c r="A67" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="1">
-        <v>75.650000000000006</v>
-      </c>
+      <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -2163,7 +2201,7 @@
         <v>29</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -2226,6 +2264,9 @@
       <c r="G72" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H72" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
@@ -2241,7 +2282,7 @@
         <v>0.49952038369304558</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -2254,7 +2295,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>22</v>
@@ -2269,7 +2310,7 @@
         <v>46</v>
       </c>
       <c r="B78" s="1">
-        <v>75.650000000000006</v>
+        <v>78.73</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2278,16 +2319,16 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B79" s="1">
-        <v>0.52505010020040077</v>
-      </c>
-      <c r="C79" s="1">
-        <v>0.50887902330743617</v>
-      </c>
-      <c r="D79" s="1">
-        <v>0.54228267297457122</v>
+        <v>24</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
@@ -2305,16 +2346,16 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B80" s="1">
-        <v>0.38764478764478771</v>
+        <v>0.52637582000000005</v>
       </c>
       <c r="C80" s="1">
-        <v>0.45471014492753631</v>
+        <v>0.50825991199999998</v>
       </c>
       <c r="D80" s="1">
-        <v>0.33781965006729481</v>
+        <v>0.545830869</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -2322,21 +2363,21 @@
         <v>29</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B81" s="1">
-        <v>0.53681431504840127</v>
+        <v>0.25914935700000002</v>
       </c>
       <c r="C81" s="1">
-        <v>0.54692169754931264</v>
+        <v>0.48880596999999998</v>
       </c>
       <c r="D81" s="1">
-        <v>0.52707373271889402</v>
+        <v>0.176312248</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -2347,18 +2388,18 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B82" s="22">
-        <v>0.89621297706174174</v>
+        <v>0.550188024</v>
       </c>
       <c r="C82" s="22">
-        <v>0.88996195493122621</v>
+        <v>0.55258570600000001</v>
       </c>
       <c r="D82" s="22">
-        <v>0.90255243371586857</v>
+        <v>0.54781106000000002</v>
       </c>
       <c r="E82" s="22"/>
       <c r="F82" s="1"/>
@@ -2366,50 +2407,627 @@
         <v>19</v>
       </c>
       <c r="H82" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B83" s="29">
-        <v>0.58855663453530505</v>
-      </c>
-      <c r="C83" s="29">
-        <v>0.60011820517887782</v>
-      </c>
-      <c r="D83" s="29">
-        <v>0.5774321223691572</v>
+        <v>6</v>
+      </c>
+      <c r="B83" s="22">
+        <v>0.89752684500000002</v>
+      </c>
+      <c r="C83" s="22">
+        <v>0.88188675599999999</v>
+      </c>
+      <c r="D83" s="22">
+        <v>0.91373169799999998</v>
       </c>
       <c r="E83" s="22"/>
       <c r="F83" s="1"/>
       <c r="G83" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H83" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B84" s="22">
-        <v>0.50823472001951941</v>
-      </c>
-      <c r="C84" s="22">
-        <v>0.5172585050906382</v>
-      </c>
-      <c r="D84" s="22">
-        <v>0.49952038369304558</v>
+        <v>16</v>
+      </c>
+      <c r="B84" s="30">
+        <v>0.57523921700000002</v>
+      </c>
+      <c r="C84" s="30">
+        <v>0.60788458599999995</v>
+      </c>
+      <c r="D84" s="30">
+        <v>0.54592146900000005</v>
       </c>
       <c r="E84" s="22"/>
       <c r="F84" s="22"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B85" s="22"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="22">
+        <v>0.50282131661442009</v>
+      </c>
+      <c r="C85" s="22">
+        <v>0.52693823915900129</v>
+      </c>
+      <c r="D85" s="22">
+        <v>0.48081534772182261</v>
+      </c>
       <c r="E85" s="22"/>
       <c r="F85" s="22"/>
+    </row>
+    <row r="88" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="12"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="28"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A89" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="J89" s="22"/>
+      <c r="K89" s="22"/>
+      <c r="L89" s="22"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A90" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" s="1">
+        <v>92.05</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="22"/>
+      <c r="L90" s="22"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J91" s="22"/>
+      <c r="K91" s="22"/>
+      <c r="L91" s="22"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.35504247440644737</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.48773189706762421</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.2791095890410959</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="22"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.29837702871410732</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.5302273987798114</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.20760043431053199</v>
+      </c>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H93" s="6">
+        <v>231</v>
+      </c>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="22"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="22">
+        <v>0.96054448249226032</v>
+      </c>
+      <c r="C94" s="22">
+        <v>0.93744657612308857</v>
+      </c>
+      <c r="D94" s="22">
+        <v>0.98480936880308301</v>
+      </c>
+      <c r="E94" s="22"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" s="6">
+        <v>8</v>
+      </c>
+      <c r="J94" s="22"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="22"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95" s="31">
+        <v>0.55976663984282804</v>
+      </c>
+      <c r="C95" s="31">
+        <v>0.65180195732350799</v>
+      </c>
+      <c r="D95" s="31">
+        <v>0.49050646405157028</v>
+      </c>
+      <c r="E95" s="22"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J95" s="22"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="22"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96" s="22">
+        <v>0.32202927538867171</v>
+      </c>
+      <c r="C96" s="22">
+        <v>0.50978698906160047</v>
+      </c>
+      <c r="D96" s="22">
+        <v>0.2353488372093023</v>
+      </c>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H96" s="6">
+        <v>128</v>
+      </c>
+      <c r="J96" s="22"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="22"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B97" s="22"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="22"/>
+      <c r="L97" s="22"/>
+    </row>
+    <row r="98" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="12"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="28"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="22"/>
+      <c r="L99" s="22"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B100" s="1">
+        <v>92.15</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="J100" s="22"/>
+      <c r="K100" s="22"/>
+      <c r="L100" s="22"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I101" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J101" s="22"/>
+      <c r="K101" s="22"/>
+      <c r="L101" s="22"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.37096079276174071</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.29486301369863022</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J102" s="22"/>
+      <c r="K102" s="22"/>
+      <c r="L102" s="22"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.22709586133710649</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.61201143946615821</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.13941368078175889</v>
+      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J103" s="22"/>
+      <c r="K103" s="22"/>
+      <c r="L103" s="22"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="22">
+        <v>0.96074275055112768</v>
+      </c>
+      <c r="C104" s="22">
+        <v>0.9338553011126155</v>
+      </c>
+      <c r="D104" s="22">
+        <v>0.98922437984061062</v>
+      </c>
+      <c r="E104" s="22"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J104" s="22"/>
+      <c r="K104" s="22"/>
+      <c r="L104" s="22"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" s="31">
+        <v>0.55962039935617103</v>
+      </c>
+      <c r="C105" s="31">
+        <v>0.68195558019292457</v>
+      </c>
+      <c r="D105" s="31">
+        <v>0.47450035810699992</v>
+      </c>
+      <c r="E105" s="22"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H105" s="6">
+        <v>256</v>
+      </c>
+      <c r="J105" s="22"/>
+      <c r="K105" s="22"/>
+      <c r="L105" s="22"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" s="22">
+        <v>0.29195804195804193</v>
+      </c>
+      <c r="C106" s="22">
+        <v>0.54240346445326593</v>
+      </c>
+      <c r="D106" s="22">
+        <v>0.19973421926910301</v>
+      </c>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="J106" s="22"/>
+      <c r="K106" s="22"/>
+      <c r="L106" s="22"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108" s="12"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="15"/>
+      <c r="I108" s="28"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A110" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B110" s="1">
+        <v>92.15</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I111" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="1">
+        <v>0.37096079276174071</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0.29486301369863022</v>
+      </c>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H112" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" s="1">
+        <v>0.22709586133710649</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.61201143946615821</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0.13941368078175889</v>
+      </c>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="22">
+        <v>0.96074275055112768</v>
+      </c>
+      <c r="C114" s="22">
+        <v>0.9338553011126155</v>
+      </c>
+      <c r="D114" s="22">
+        <v>0.98922437984061062</v>
+      </c>
+      <c r="E114" s="22"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="31">
+        <v>0.55962039935617103</v>
+      </c>
+      <c r="C115" s="31">
+        <v>0.68195558019292457</v>
+      </c>
+      <c r="D115" s="31">
+        <v>0.47450035810699992</v>
+      </c>
+      <c r="E115" s="22"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H115" s="6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" s="22">
+        <v>0.29195804195804193</v>
+      </c>
+      <c r="C116" s="22">
+        <v>0.54240346445326593</v>
+      </c>
+      <c r="D116" s="22">
+        <v>0.19973421926910301</v>
+      </c>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B117" s="22"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B118" s="22"/>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>